<commit_message>
Documentation:     + Update documentation RTL:     + Change CLR bit position in CFG for each channels to clarify prog model and help with header generation
</commit_message>
<xml_diff>
--- a/docs/I2C_reference.xlsx
+++ b/docs/I2C_reference.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Info " sheetId="1" state="visible" r:id="rId2"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="320">
   <si>
     <t xml:space="preserve">Document Information</t>
   </si>
@@ -622,10 +622,37 @@
     <t xml:space="preserve">uDMA TX I2C stream configuration register.</t>
   </si>
   <si>
+    <t xml:space="preserve">CMD_SADDR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uDMA CMD I2C buffer base address configuration register.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CMD_SIZE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uDMA CMD I2C buffer size configuration register.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CMD_CFG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uDMA CMD I2C stream configuration register.</t>
+  </si>
+  <si>
     <t xml:space="preserve">STATUS</t>
   </si>
   <si>
-    <t xml:space="preserve">0x20</t>
+    <t xml:space="preserve">0x30</t>
   </si>
   <si>
     <t xml:space="preserve">W</t>
@@ -637,7 +664,7 @@
     <t xml:space="preserve">SETUP</t>
   </si>
   <si>
-    <t xml:space="preserve">0x24</t>
+    <t xml:space="preserve">0x34</t>
   </si>
   <si>
     <t xml:space="preserve">R</t>
@@ -683,20 +710,20 @@
 This signal is used also to queue a transfer if one is already ongoing.</t>
   </si>
   <si>
+    <t xml:space="preserve">PENDING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RX transfer pending in queue status flag:
+-1'b0: no pending transfer in the queue
+-1'b1: pending transfer in the queue</t>
+  </si>
+  <si>
     <t xml:space="preserve">CLR</t>
   </si>
   <si>
     <t xml:space="preserve">RX channel clear and stop transfer:
 -1'b0: disable
 -1'b1: stop and clear the on-going transfer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PENDING</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RX transfer pending in queue status flag:
--1'b0: no pending transfer in the queue
--1'b1: pending transfer in the queue</t>
   </si>
   <si>
     <t xml:space="preserve">TX buffer base address bitfield:
@@ -721,14 +748,46 @@
 This signal is used also to queue a transfer if one is already ongoing.</t>
   </si>
   <si>
+    <t xml:space="preserve">TX transfer pending in queue status flag:
+-1'b0: no pending transfer in the queue
+-1'b1: pending transfer in the queue</t>
+  </si>
+  <si>
     <t xml:space="preserve">TX channel clear and stop transfer bitfield:
 -1'b0: disabled
 -1'b1: stop and clear the on-going transfer</t>
   </si>
   <si>
-    <t xml:space="preserve">TX transfer pending in queue status flag:
+    <t xml:space="preserve">CMD buffer base address bitfield:
+- Read: returns value of the buffer pointer until transfer is finished. Else returns 0.
+- Write: sets buffer base address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CMD buffer size bitfield in bytes. (128kBytes maximum)
+- Read: returns remaining buffer size to transfer.
+- Write: sets buffer size.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CMD channel continuous mode bitfield:
+-1'b0: disabled
+-1'b1: enabled
+At the end of the buffer transfer, the uDMA reloads the address / buffer size and starts a new transfer.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CMD channel enable and start transfer bitfield:
+-1'b0: disabled
+-1'b1: enable and start the transfer
+This signal is used also to queue a transfer if one is already ongoing.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CMD transfer pending in queue status flag:
 -1'b0: no pending transfer in the queue
 -1'b1: pending transfer in the queue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CMD channel clear and stop transfer bitfield:
+-1'b0: disabled
+-1'b1: stop and clear the on-going transfer</t>
   </si>
   <si>
     <t xml:space="preserve">BUSY</t>
@@ -756,7 +815,7 @@
     <t xml:space="preserve">Command name</t>
   </si>
   <si>
-    <t xml:space="preserve">Command number</t>
+    <t xml:space="preserve">Command field</t>
   </si>
   <si>
     <t xml:space="preserve">Parameter</t>
@@ -816,21 +875,24 @@
     <t xml:space="preserve">The value following the I2C_CMD_WAIT command indicates I2C dummy clock cycles value.</t>
   </si>
   <si>
+    <t xml:space="preserve">2 bytes(bit[15:0])</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I2C wait dummy cycles command.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I2C_CMD_RPT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0xC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The value following the I2C_CMD_RPT command indicates number of times to repeat next command.</t>
+  </si>
+  <si>
     <t xml:space="preserve">1 byte.</t>
   </si>
   <si>
-    <t xml:space="preserve">I2C wait dummy cycles command.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I2C_CMD_RPT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0xC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The value following the I2C_CMD_RPT command indicates number of times to repeat next command.</t>
-  </si>
-  <si>
     <t xml:space="preserve">I2C next command repeat command.</t>
   </si>
   <si>
@@ -840,7 +902,7 @@
     <t xml:space="preserve">0xE</t>
   </si>
   <si>
-    <t xml:space="preserve">The value following the I2C_CMD_CFG command indicates I2C clock divider 16bits value related to SoC clock frequency. MSB byte is sent first.</t>
+    <t xml:space="preserve">The value following the I2C_CMD_CFG command indicates I2C clock divider 16bits value related to SoC clock frequency.</t>
   </si>
   <si>
     <t xml:space="preserve">2 bytes.</t>
@@ -864,13 +926,157 @@
     <t xml:space="preserve">I2C wait uDMA external event command.</t>
   </si>
   <si>
-    <t xml:space="preserve">Parameter Bit field</t>
+    <t xml:space="preserve">I2C_CMD_WRB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The value in the lowest byte will be sent on the bus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 byte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I2C write byte command</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I2C_CMD_EOT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Signal end of transfer (next transfer may be en-queued)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I2C_CMD_SETUP_UCA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bit 27 describe if read or write / bits[23:0] are the buffer(tx or rx) address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1(bit[27]) + 24(bit[23:0])</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Setup RX or TX channel start address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I2C_CMD_SETUP_UCS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bit 27 describe if read or write / bits[15:0] are the buffer(tx or rx) size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1(bit27) + 15(bit[15:0]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Setup RX or TX channel transfer size+enable channel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parameter bit field</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Field value</t>
   </si>
   <si>
     <t xml:space="preserve">I2C_CMD</t>
   </si>
   <si>
+    <t xml:space="preserve">DUMMY_CYCLES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ARG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dummy cycles to wait</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RPT_NB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">number of repeats to do</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CFG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I2C configuration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DATA_BYTE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">byte to be written</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I2C rx/tx channel address configuration command </t>
+  </si>
+  <si>
+    <t xml:space="preserve">TXRXN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tx/rx selection (tx if 1, rx if 0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SADDR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rx/tx channel start address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I2C rx/tx channel transfer size configuration command </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SIZE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rx/tx channel transfer size</t>
+  </si>
+  <si>
     <t xml:space="preserve">testcase location&amp;name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reg test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test default value and rw access to all registers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Read byte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">read a byte from device (eprom)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">write byte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">write a byte to device (eprom)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Read chain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">read a chain of bytes from device (eprom)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">write chain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">write a chain of bytes to device (eprom)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wait events</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wait on event propagated by uDMA</t>
   </si>
 </sst>
 </file>
@@ -1097,7 +1303,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="68">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1352,10 +1558,6 @@
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1687,33 +1889,81 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="6.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="41.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="30.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="10.27"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="67" t="s">
+      <c r="A1" s="66" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="67" t="s">
+      <c r="B1" s="66" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="67" t="s">
-        <v>255</v>
-      </c>
-      <c r="D1" s="67" t="s">
+      <c r="C1" s="66" t="s">
+        <v>307</v>
+      </c>
+      <c r="D1" s="66" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>308</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B4" s="34" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>314</v>
+      </c>
+      <c r="B5" s="34" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>316</v>
+      </c>
+      <c r="B6" s="34" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>318</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>319</v>
       </c>
     </row>
   </sheetData>
@@ -2165,7 +2415,7 @@
   </sheetPr>
   <dimension ref="A1:AC44"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A28" activeCellId="0" sqref="A28"/>
     </sheetView>
   </sheetViews>
@@ -2825,7 +3075,7 @@
   </sheetPr>
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -2871,12 +3121,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
+      <selection pane="bottomLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3083,7 +3333,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="57" t="s">
         <v>183</v>
       </c>
@@ -3094,28 +3344,27 @@
         <v>32</v>
       </c>
       <c r="E8" s="58" t="s">
-        <v>9</v>
+        <v>165</v>
       </c>
       <c r="F8" s="58" t="s">
         <v>166</v>
       </c>
       <c r="G8" s="58" t="s">
-        <v>185</v>
+        <v>166</v>
       </c>
       <c r="H8" s="58" t="s">
         <v>164</v>
       </c>
       <c r="I8" s="54" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="57" t="s">
         <v>186</v>
       </c>
-      <c r="J8" s="58"/>
-    </row>
-    <row r="9" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="57" t="s">
+      <c r="C9" s="58" t="s">
         <v>187</v>
-      </c>
-      <c r="C9" s="58" t="s">
-        <v>188</v>
       </c>
       <c r="D9" s="57" t="n">
         <v>32</v>
@@ -3127,13 +3376,92 @@
         <v>166</v>
       </c>
       <c r="G9" s="58" t="s">
-        <v>189</v>
+        <v>166</v>
       </c>
       <c r="H9" s="58" t="s">
         <v>164</v>
       </c>
       <c r="I9" s="54" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="57" t="s">
+        <v>189</v>
+      </c>
+      <c r="C10" s="58" t="s">
         <v>190</v>
+      </c>
+      <c r="D10" s="57" t="n">
+        <v>32</v>
+      </c>
+      <c r="E10" s="58" t="s">
+        <v>165</v>
+      </c>
+      <c r="F10" s="58" t="s">
+        <v>166</v>
+      </c>
+      <c r="G10" s="58" t="s">
+        <v>166</v>
+      </c>
+      <c r="H10" s="58" t="s">
+        <v>164</v>
+      </c>
+      <c r="I10" s="54" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="57" t="s">
+        <v>192</v>
+      </c>
+      <c r="C11" s="58" t="s">
+        <v>193</v>
+      </c>
+      <c r="D11" s="57" t="n">
+        <v>32</v>
+      </c>
+      <c r="E11" s="58" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="58" t="s">
+        <v>166</v>
+      </c>
+      <c r="G11" s="58" t="s">
+        <v>194</v>
+      </c>
+      <c r="H11" s="58" t="s">
+        <v>164</v>
+      </c>
+      <c r="I11" s="54" t="s">
+        <v>195</v>
+      </c>
+      <c r="J11" s="58"/>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="57" t="s">
+        <v>196</v>
+      </c>
+      <c r="C12" s="58" t="s">
+        <v>197</v>
+      </c>
+      <c r="D12" s="57" t="n">
+        <v>32</v>
+      </c>
+      <c r="E12" s="58" t="s">
+        <v>165</v>
+      </c>
+      <c r="F12" s="58" t="s">
+        <v>166</v>
+      </c>
+      <c r="G12" s="58" t="s">
+        <v>198</v>
+      </c>
+      <c r="H12" s="58" t="s">
+        <v>164</v>
+      </c>
+      <c r="I12" s="54" t="s">
+        <v>199</v>
       </c>
     </row>
   </sheetData>
@@ -3158,12 +3486,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H27"/>
+  <dimension ref="A1:H1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="H14" activeCellId="0" sqref="H14"/>
+      <selection pane="bottomLeft" activeCell="H19" activeCellId="0" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3181,13 +3509,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="59" t="s">
-        <v>191</v>
+        <v>200</v>
       </c>
       <c r="B1" s="42" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="C1" s="42" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
       <c r="D1" s="42" t="s">
         <v>79</v>
@@ -3205,7 +3533,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="43.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="60" t="s">
         <v>163</v>
       </c>
@@ -3216,7 +3544,7 @@
         <v>0</v>
       </c>
       <c r="D2" s="52" t="n">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="E2" s="58" t="s">
         <v>166</v>
@@ -3228,10 +3556,10 @@
         <v>164</v>
       </c>
       <c r="H2" s="62" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="43.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="60" t="s">
         <v>168</v>
       </c>
@@ -3242,7 +3570,7 @@
         <v>0</v>
       </c>
       <c r="D3" s="52" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E3" s="58" t="s">
         <v>166</v>
@@ -3254,12 +3582,12 @@
         <v>164</v>
       </c>
       <c r="H3" s="62" t="s">
-        <v>195</v>
+        <v>204</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="72.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="60" t="s">
-        <v>196</v>
+        <v>205</v>
       </c>
       <c r="B4" s="58" t="s">
         <v>171</v>
@@ -3280,12 +3608,12 @@
         <v>164</v>
       </c>
       <c r="H4" s="62" t="s">
-        <v>197</v>
+        <v>206</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="58" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="60" t="s">
-        <v>198</v>
+        <v>207</v>
       </c>
       <c r="B5" s="58" t="s">
         <v>171</v>
@@ -3306,12 +3634,12 @@
         <v>164</v>
       </c>
       <c r="H5" s="62" t="s">
-        <v>199</v>
+        <v>208</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="43.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="60" t="s">
-        <v>200</v>
+        <v>209</v>
       </c>
       <c r="B6" s="58" t="s">
         <v>171</v>
@@ -3323,45 +3651,45 @@
         <v>1</v>
       </c>
       <c r="E6" s="58" t="s">
-        <v>185</v>
+        <v>198</v>
       </c>
       <c r="F6" s="52" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="G6" s="61" t="s">
         <v>164</v>
       </c>
       <c r="H6" s="62" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="43.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="32.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="60" t="s">
-        <v>202</v>
+        <v>211</v>
       </c>
       <c r="B7" s="58" t="s">
         <v>171</v>
       </c>
       <c r="C7" s="52" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D7" s="52" t="n">
         <v>1</v>
       </c>
       <c r="E7" s="58" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="F7" s="52" t="s">
-        <v>185</v>
+        <v>198</v>
       </c>
       <c r="G7" s="61" t="s">
         <v>164</v>
       </c>
       <c r="H7" s="62" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="43.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="60" t="s">
         <v>174</v>
       </c>
@@ -3372,7 +3700,7 @@
         <v>0</v>
       </c>
       <c r="D8" s="52" t="n">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="E8" s="58" t="s">
         <v>166</v>
@@ -3384,7 +3712,7 @@
         <v>164</v>
       </c>
       <c r="H8" s="62" t="s">
-        <v>204</v>
+        <v>213</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="43.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3398,7 +3726,7 @@
         <v>0</v>
       </c>
       <c r="D9" s="52" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E9" s="58" t="s">
         <v>166</v>
@@ -3410,12 +3738,12 @@
         <v>164</v>
       </c>
       <c r="H9" s="62" t="s">
-        <v>205</v>
+        <v>214</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="72.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="60" t="s">
-        <v>196</v>
+        <v>205</v>
       </c>
       <c r="B10" s="58" t="s">
         <v>180</v>
@@ -3436,12 +3764,12 @@
         <v>164</v>
       </c>
       <c r="H10" s="62" t="s">
-        <v>206</v>
+        <v>215</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="58" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="60" t="s">
-        <v>198</v>
+        <v>207</v>
       </c>
       <c r="B11" s="58" t="s">
         <v>180</v>
@@ -3462,12 +3790,12 @@
         <v>164</v>
       </c>
       <c r="H11" s="62" t="s">
-        <v>207</v>
+        <v>216</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="43.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="60" t="s">
-        <v>200</v>
+        <v>209</v>
       </c>
       <c r="B12" s="58" t="s">
         <v>180</v>
@@ -3479,47 +3807,47 @@
         <v>1</v>
       </c>
       <c r="E12" s="58" t="s">
-        <v>185</v>
+        <v>198</v>
       </c>
       <c r="F12" s="52" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="G12" s="61" t="s">
         <v>164</v>
       </c>
       <c r="H12" s="62" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="43.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="32.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="60" t="s">
-        <v>202</v>
+        <v>211</v>
       </c>
       <c r="B13" s="58" t="s">
         <v>180</v>
       </c>
       <c r="C13" s="52" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D13" s="52" t="n">
         <v>1</v>
       </c>
       <c r="E13" s="58" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="F13" s="52" t="s">
-        <v>185</v>
+        <v>198</v>
       </c>
       <c r="G13" s="61" t="s">
         <v>164</v>
       </c>
       <c r="H13" s="62" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="43.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>210</v>
+        <v>218</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="60" t="s">
+        <v>183</v>
       </c>
       <c r="B14" s="58" t="s">
         <v>183</v>
@@ -3528,53 +3856,53 @@
         <v>0</v>
       </c>
       <c r="D14" s="52" t="n">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="E14" s="58" t="s">
         <v>166</v>
       </c>
-      <c r="F14" s="58" t="s">
-        <v>185</v>
-      </c>
-      <c r="G14" s="43" t="s">
+      <c r="F14" s="52" t="s">
+        <v>166</v>
+      </c>
+      <c r="G14" s="61" t="s">
         <v>164</v>
       </c>
       <c r="H14" s="62" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="43.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="60" t="s">
-        <v>212</v>
+        <v>186</v>
       </c>
       <c r="B15" s="58" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="C15" s="52" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D15" s="52" t="n">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="E15" s="58" t="s">
         <v>166</v>
       </c>
-      <c r="F15" s="58" t="s">
-        <v>185</v>
-      </c>
-      <c r="G15" s="43" t="s">
+      <c r="F15" s="52" t="s">
+        <v>166</v>
+      </c>
+      <c r="G15" s="61" t="s">
         <v>164</v>
       </c>
       <c r="H15" s="62" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="53.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="60" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="B16" s="58" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="C16" s="52" t="n">
         <v>0</v>
@@ -3582,116 +3910,196 @@
       <c r="D16" s="52" t="n">
         <v>1</v>
       </c>
-      <c r="E16" s="61" t="s">
+      <c r="E16" s="58" t="s">
         <v>166</v>
       </c>
-      <c r="F16" s="61" t="s">
+      <c r="F16" s="52" t="s">
+        <v>166</v>
+      </c>
+      <c r="G16" s="61" t="s">
+        <v>164</v>
+      </c>
+      <c r="H16" s="62" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="43.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="60" t="s">
+        <v>207</v>
+      </c>
+      <c r="B17" s="58" t="s">
         <v>189</v>
       </c>
-      <c r="G16" s="43" t="s">
+      <c r="C17" s="52" t="n">
+        <v>4</v>
+      </c>
+      <c r="D17" s="52" t="n">
+        <v>1</v>
+      </c>
+      <c r="E17" s="58" t="s">
+        <v>166</v>
+      </c>
+      <c r="F17" s="52" t="s">
+        <v>166</v>
+      </c>
+      <c r="G17" s="61" t="s">
         <v>164</v>
       </c>
-      <c r="H16" s="62" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="60"/>
-      <c r="B17" s="52"/>
-      <c r="C17" s="43"/>
-      <c r="D17" s="43"/>
-      <c r="E17" s="61"/>
-      <c r="F17" s="61"/>
-      <c r="G17" s="43"/>
-      <c r="H17" s="63"/>
-    </row>
-    <row r="18" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="60"/>
-      <c r="B18" s="52"/>
-      <c r="C18" s="43"/>
-      <c r="D18" s="43"/>
-      <c r="E18" s="61"/>
-      <c r="F18" s="61"/>
-      <c r="G18" s="43"/>
-      <c r="H18" s="63"/>
-    </row>
-    <row r="19" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="52"/>
-      <c r="C19" s="43"/>
-      <c r="D19" s="64"/>
-      <c r="E19" s="61"/>
-      <c r="F19" s="61"/>
-      <c r="G19" s="43"/>
-      <c r="H19" s="63"/>
-    </row>
-    <row r="20" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="52"/>
-      <c r="C20" s="43"/>
-      <c r="D20" s="61"/>
-      <c r="E20" s="61"/>
-      <c r="F20" s="61"/>
-      <c r="G20" s="43"/>
-      <c r="H20" s="63"/>
-    </row>
-    <row r="21" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="52"/>
-      <c r="C21" s="43"/>
-      <c r="D21" s="43"/>
-      <c r="E21" s="61"/>
-      <c r="F21" s="61"/>
-      <c r="G21" s="43"/>
-      <c r="H21" s="63"/>
-    </row>
-    <row r="22" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="52"/>
-      <c r="C22" s="43"/>
-      <c r="D22" s="43"/>
-      <c r="E22" s="61"/>
-      <c r="F22" s="61"/>
-      <c r="G22" s="43"/>
-      <c r="H22" s="63"/>
+      <c r="H17" s="62" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="32.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="60" t="s">
+        <v>209</v>
+      </c>
+      <c r="B18" s="58" t="s">
+        <v>189</v>
+      </c>
+      <c r="C18" s="52" t="n">
+        <v>5</v>
+      </c>
+      <c r="D18" s="52" t="n">
+        <v>1</v>
+      </c>
+      <c r="E18" s="58" t="s">
+        <v>198</v>
+      </c>
+      <c r="F18" s="52" t="s">
+        <v>194</v>
+      </c>
+      <c r="G18" s="61" t="s">
+        <v>164</v>
+      </c>
+      <c r="H18" s="62" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="32.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="60" t="s">
+        <v>211</v>
+      </c>
+      <c r="B19" s="58" t="s">
+        <v>189</v>
+      </c>
+      <c r="C19" s="52" t="n">
+        <v>6</v>
+      </c>
+      <c r="D19" s="52" t="n">
+        <v>1</v>
+      </c>
+      <c r="E19" s="58" t="s">
+        <v>194</v>
+      </c>
+      <c r="F19" s="52" t="s">
+        <v>198</v>
+      </c>
+      <c r="G19" s="61" t="s">
+        <v>164</v>
+      </c>
+      <c r="H19" s="62" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="32.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>225</v>
+      </c>
+      <c r="B20" s="58" t="s">
+        <v>192</v>
+      </c>
+      <c r="C20" s="52" t="n">
+        <v>0</v>
+      </c>
+      <c r="D20" s="52" t="n">
+        <v>1</v>
+      </c>
+      <c r="E20" s="58" t="s">
+        <v>166</v>
+      </c>
+      <c r="F20" s="58" t="s">
+        <v>194</v>
+      </c>
+      <c r="G20" s="43" t="s">
+        <v>164</v>
+      </c>
+      <c r="H20" s="62" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="32.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="60" t="s">
+        <v>227</v>
+      </c>
+      <c r="B21" s="58" t="s">
+        <v>192</v>
+      </c>
+      <c r="C21" s="52" t="n">
+        <v>1</v>
+      </c>
+      <c r="D21" s="52" t="n">
+        <v>1</v>
+      </c>
+      <c r="E21" s="58" t="s">
+        <v>166</v>
+      </c>
+      <c r="F21" s="58" t="s">
+        <v>194</v>
+      </c>
+      <c r="G21" s="43" t="s">
+        <v>164</v>
+      </c>
+      <c r="H21" s="62" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="22.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="60" t="s">
+        <v>229</v>
+      </c>
+      <c r="B22" s="58" t="s">
+        <v>196</v>
+      </c>
+      <c r="C22" s="52" t="n">
+        <v>0</v>
+      </c>
+      <c r="D22" s="52" t="n">
+        <v>1</v>
+      </c>
+      <c r="E22" s="61" t="s">
+        <v>166</v>
+      </c>
+      <c r="F22" s="61" t="s">
+        <v>198</v>
+      </c>
+      <c r="G22" s="43" t="s">
+        <v>164</v>
+      </c>
+      <c r="H22" s="62" t="s">
+        <v>230</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C23" s="43"/>
-      <c r="D23" s="64"/>
+      <c r="D23" s="43"/>
       <c r="E23" s="61"/>
       <c r="F23" s="61"/>
       <c r="G23" s="43"/>
       <c r="H23" s="63"/>
     </row>
-    <row r="24" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B24" s="52"/>
       <c r="C24" s="43"/>
-      <c r="D24" s="61"/>
+      <c r="D24" s="43"/>
       <c r="E24" s="61"/>
       <c r="F24" s="61"/>
       <c r="G24" s="43"/>
-      <c r="H24" s="63"/>
-    </row>
-    <row r="25" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C25" s="43"/>
-      <c r="D25" s="43"/>
-      <c r="E25" s="61"/>
-      <c r="F25" s="61"/>
-      <c r="G25" s="43"/>
-      <c r="H25" s="63"/>
-    </row>
-    <row r="26" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C26" s="43"/>
-      <c r="D26" s="43"/>
-      <c r="E26" s="61"/>
-      <c r="F26" s="61"/>
-      <c r="G26" s="43"/>
-      <c r="H26" s="63"/>
-    </row>
-    <row r="27" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B27" s="52"/>
-      <c r="C27" s="43"/>
-      <c r="D27" s="43"/>
-      <c r="E27" s="61"/>
-      <c r="F27" s="61"/>
-      <c r="G27" s="43"/>
-      <c r="H27" s="65"/>
-    </row>
+      <c r="H24" s="64"/>
+    </row>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -3708,10 +4116,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3719,186 +4127,260 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="52" width="12.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="52" width="18.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="66" width="43.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="65" width="43.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="52" width="34.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="78.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="67" t="s">
-        <v>216</v>
+      <c r="A1" s="66" t="s">
+        <v>231</v>
       </c>
       <c r="B1" s="42" t="s">
         <v>79</v>
       </c>
       <c r="C1" s="42" t="s">
-        <v>217</v>
-      </c>
-      <c r="D1" s="68" t="s">
-        <v>218</v>
+        <v>232</v>
+      </c>
+      <c r="D1" s="67" t="s">
+        <v>233</v>
       </c>
       <c r="E1" s="42" t="s">
-        <v>219</v>
-      </c>
-      <c r="F1" s="67" t="s">
+        <v>234</v>
+      </c>
+      <c r="F1" s="66" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>220</v>
+        <v>235</v>
       </c>
       <c r="B2" s="52" t="n">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="C2" s="52" t="s">
         <v>164</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>221</v>
+        <v>236</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>222</v>
+        <v>237</v>
       </c>
       <c r="B3" s="52" t="n">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="C3" s="52" t="s">
-        <v>223</v>
+        <v>238</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>224</v>
+        <v>239</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>225</v>
+        <v>240</v>
       </c>
       <c r="B4" s="52" t="n">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="C4" s="52" t="s">
         <v>169</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>226</v>
+        <v>241</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>227</v>
+        <v>242</v>
       </c>
       <c r="B5" s="52" t="n">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="C5" s="52" t="s">
-        <v>228</v>
+        <v>243</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>229</v>
+        <v>244</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="58" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>230</v>
+        <v>245</v>
       </c>
       <c r="B6" s="52" t="n">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="C6" s="52" t="s">
         <v>172</v>
       </c>
       <c r="D6" s="57" t="s">
-        <v>231</v>
+        <v>246</v>
       </c>
       <c r="E6" s="58" t="s">
-        <v>232</v>
+        <v>247</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>233</v>
+        <v>248</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>234</v>
+        <v>249</v>
       </c>
       <c r="B7" s="52" t="n">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="C7" s="52" t="s">
-        <v>235</v>
+        <v>250</v>
       </c>
       <c r="D7" s="57" t="s">
-        <v>236</v>
+        <v>251</v>
       </c>
       <c r="E7" s="52" t="s">
-        <v>237</v>
+        <v>252</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="43.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>239</v>
+        <v>254</v>
       </c>
       <c r="B8" s="52" t="n">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="C8" s="43" t="s">
-        <v>240</v>
+        <v>255</v>
       </c>
       <c r="D8" s="57" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="E8" s="52" t="s">
-        <v>237</v>
+        <v>257</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="43.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>243</v>
+        <v>259</v>
       </c>
       <c r="B9" s="52" t="n">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="C9" s="52" t="s">
-        <v>244</v>
+        <v>260</v>
       </c>
       <c r="D9" s="57" t="s">
-        <v>245</v>
+        <v>261</v>
       </c>
       <c r="E9" s="52" t="s">
-        <v>246</v>
+        <v>262</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>247</v>
+        <v>263</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="43.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>248</v>
+        <v>264</v>
       </c>
       <c r="B10" s="52" t="n">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="C10" s="43" t="s">
-        <v>249</v>
+        <v>265</v>
       </c>
       <c r="D10" s="57" t="s">
-        <v>250</v>
+        <v>266</v>
       </c>
       <c r="E10" s="52" t="s">
-        <v>251</v>
+        <v>267</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>252</v>
+        <v>268</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>269</v>
+      </c>
+      <c r="B11" s="52" t="n">
+        <v>32</v>
+      </c>
+      <c r="C11" s="52" t="s">
+        <v>270</v>
+      </c>
+      <c r="D11" s="65" t="s">
+        <v>271</v>
+      </c>
+      <c r="E11" s="52" t="s">
+        <v>272</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>274</v>
+      </c>
+      <c r="B12" s="52" t="n">
+        <v>32</v>
+      </c>
+      <c r="C12" s="52" t="s">
+        <v>275</v>
+      </c>
+      <c r="F12" s="0" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>277</v>
+      </c>
+      <c r="B13" s="52" t="n">
+        <v>32</v>
+      </c>
+      <c r="C13" s="52" t="s">
+        <v>278</v>
+      </c>
+      <c r="D13" s="65" t="s">
+        <v>279</v>
+      </c>
+      <c r="E13" s="52" t="s">
+        <v>280</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>282</v>
+      </c>
+      <c r="B14" s="52" t="n">
+        <v>32</v>
+      </c>
+      <c r="C14" s="52" t="s">
+        <v>283</v>
+      </c>
+      <c r="D14" s="65" t="s">
+        <v>284</v>
+      </c>
+      <c r="E14" s="52" t="s">
+        <v>285</v>
+      </c>
+      <c r="F14" s="0" t="s">
+        <v>286</v>
       </c>
     </row>
   </sheetData>
@@ -3917,190 +4399,461 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="33" width="74.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="74.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="33" width="74.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="8.67"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="59" t="s">
-        <v>253</v>
+        <v>287</v>
       </c>
       <c r="B1" s="42" t="s">
-        <v>216</v>
+        <v>231</v>
       </c>
       <c r="C1" s="42" t="s">
-        <v>193</v>
+        <v>105</v>
       </c>
       <c r="D1" s="42" t="s">
         <v>79</v>
       </c>
-      <c r="E1" s="55" t="s">
+      <c r="E1" s="42" t="s">
+        <v>288</v>
+      </c>
+      <c r="F1" s="55" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>254</v>
+        <v>289</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>220</v>
+        <v>235</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="D2" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="E2" s="33" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>4</v>
+      </c>
+      <c r="E2" s="43" t="s">
+        <v>164</v>
+      </c>
+      <c r="F2" s="33" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>254</v>
+        <v>289</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>222</v>
+        <v>237</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="D3" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="E3" s="33" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>4</v>
+      </c>
+      <c r="E3" s="43" t="s">
+        <v>238</v>
+      </c>
+      <c r="F3" s="33" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>254</v>
+        <v>289</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>225</v>
+        <v>240</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="D4" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="E4" s="33" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>4</v>
+      </c>
+      <c r="E4" s="43" t="s">
+        <v>169</v>
+      </c>
+      <c r="F4" s="33" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>254</v>
+        <v>289</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>227</v>
+        <v>242</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="D5" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="E5" s="33" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>4</v>
+      </c>
+      <c r="E5" s="43" t="s">
+        <v>243</v>
+      </c>
+      <c r="F5" s="33" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>254</v>
+        <v>289</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>230</v>
+        <v>245</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="E6" s="33" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>4</v>
+      </c>
+      <c r="E6" s="43" t="s">
+        <v>172</v>
+      </c>
+      <c r="F6" s="33" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>254</v>
+        <v>289</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>234</v>
+        <v>249</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="D7" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="E7" s="33" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>4</v>
+      </c>
+      <c r="E7" s="43" t="s">
+        <v>250</v>
+      </c>
+      <c r="F7" s="33" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>254</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>239</v>
+        <v>290</v>
+      </c>
+      <c r="B8" s="34" t="s">
+        <v>249</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>0</v>
       </c>
       <c r="D8" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="E8" s="33" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>16</v>
+      </c>
+      <c r="E8" s="43" t="s">
+        <v>291</v>
+      </c>
+      <c r="F8" s="33" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
+        <v>289</v>
+      </c>
+      <c r="B9" s="0" t="s">
         <v>254</v>
       </c>
-      <c r="B9" s="0" t="s">
-        <v>243</v>
-      </c>
       <c r="C9" s="0" t="n">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="D9" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="E9" s="33" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>4</v>
+      </c>
+      <c r="E9" s="43" t="s">
+        <v>255</v>
+      </c>
+      <c r="F9" s="33" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
+        <v>293</v>
+      </c>
+      <c r="B10" s="34" t="s">
         <v>254</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>248</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>0</v>
       </c>
       <c r="D10" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="E10" s="43" t="s">
+        <v>291</v>
+      </c>
+      <c r="F10" s="33" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>289</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>259</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="E11" s="43" t="s">
+        <v>260</v>
+      </c>
+      <c r="F11" s="33" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>295</v>
+      </c>
+      <c r="B12" s="34" t="s">
+        <v>259</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="E12" s="43" t="s">
+        <v>291</v>
+      </c>
+      <c r="F12" s="33" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>289</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>264</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="E13" s="43" t="s">
+        <v>265</v>
+      </c>
+      <c r="F13" s="33" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>289</v>
+      </c>
+      <c r="B14" s="34" t="s">
+        <v>269</v>
+      </c>
+      <c r="C14" s="34" t="n">
+        <v>28</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="E14" s="43" t="s">
+        <v>270</v>
+      </c>
+      <c r="F14" s="33" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>297</v>
+      </c>
+      <c r="B15" s="34" t="s">
+        <v>269</v>
+      </c>
+      <c r="C15" s="34" t="n">
+        <v>0</v>
+      </c>
+      <c r="D15" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="E10" s="33" t="s">
-        <v>252</v>
+      <c r="E15" s="43" t="s">
+        <v>291</v>
+      </c>
+      <c r="F15" s="33" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>289</v>
+      </c>
+      <c r="B16" s="34" t="s">
+        <v>274</v>
+      </c>
+      <c r="C16" s="34" t="n">
+        <v>28</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="E16" s="43" t="s">
+        <v>275</v>
+      </c>
+      <c r="F16" s="33" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>289</v>
+      </c>
+      <c r="B17" s="34" t="s">
+        <v>277</v>
+      </c>
+      <c r="C17" s="34" t="n">
+        <v>28</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="E17" s="43" t="s">
+        <v>278</v>
+      </c>
+      <c r="F17" s="33" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>300</v>
+      </c>
+      <c r="B18" s="34" t="s">
+        <v>277</v>
+      </c>
+      <c r="C18" s="34" t="n">
+        <v>27</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E18" s="43" t="s">
+        <v>291</v>
+      </c>
+      <c r="F18" s="33" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>302</v>
+      </c>
+      <c r="B19" s="34" t="s">
+        <v>277</v>
+      </c>
+      <c r="C19" s="34" t="n">
+        <v>0</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="E19" s="43" t="s">
+        <v>291</v>
+      </c>
+      <c r="F19" s="33" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>289</v>
+      </c>
+      <c r="B20" s="34" t="s">
+        <v>282</v>
+      </c>
+      <c r="C20" s="34" t="n">
+        <v>28</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="E20" s="43" t="s">
+        <v>283</v>
+      </c>
+      <c r="F20" s="57" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>300</v>
+      </c>
+      <c r="B21" s="34" t="s">
+        <v>282</v>
+      </c>
+      <c r="C21" s="34" t="n">
+        <v>27</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E21" s="43" t="s">
+        <v>291</v>
+      </c>
+      <c r="F21" s="33" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="B22" s="34" t="s">
+        <v>282</v>
+      </c>
+      <c r="C22" s="34" t="n">
+        <v>0</v>
+      </c>
+      <c r="D22" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="E22" s="43" t="s">
+        <v>291</v>
+      </c>
+      <c r="F22" s="33" t="s">
+        <v>306</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add ACK flag in STATUS register for polling
</commit_message>
<xml_diff>
--- a/docs/I2C_reference.xlsx
+++ b/docs/I2C_reference.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="8"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Info " sheetId="1" state="visible" r:id="rId2"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="322">
   <si>
     <t xml:space="preserve">Document Information</t>
   </si>
@@ -804,6 +804,14 @@
     <t xml:space="preserve">I2C arbitration lost status flag:
 - 1'b0: no error
 - 1'b1: arbitration lost error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ACK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I2C ack flag, can be polling for busy:
+- 1'b0: ACK
+- 1'b1: NAK</t>
   </si>
   <si>
     <t xml:space="preserve">DO_RST</t>
@@ -1656,16 +1664,16 @@
   </sheetPr>
   <dimension ref="B3:D30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B26" activeCellId="0" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="39.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.67"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.5204081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="39.280612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1876,7 +1884,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1891,17 +1899,17 @@
   </sheetPr>
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="41.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="30.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="10.27"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="41.4438775510204"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.5102040816327"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.3265306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.1224489795918"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1912,7 +1920,7 @@
         <v>11</v>
       </c>
       <c r="C1" s="66" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="D1" s="66" t="s">
         <v>9</v>
@@ -1920,56 +1928,56 @@
     </row>
     <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="B4" s="34" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="B5" s="34" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="B6" s="34" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1984,17 +1992,17 @@
   </sheetPr>
   <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="42.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="29.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="10.27"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.5459183673469"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="41.8469387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.0255102040816"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.1224489795918"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2320,7 +2328,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2335,17 +2343,17 @@
   </sheetPr>
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="44.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="3" style="0" width="10.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="24.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="10.27"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="44.0051020408163"/>
+    <col collapsed="false" hidden="false" max="6" min="3" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="24.4336734693878"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.1224489795918"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2400,7 +2408,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2415,21 +2423,21 @@
   </sheetPr>
   <dimension ref="A1:AC44"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A28" activeCellId="0" sqref="A28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="2" style="0" width="8.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="19.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="11.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="11" style="0" width="8.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="10.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="16" style="0" width="8.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="10.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="23" style="0" width="8.67"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="8" min="2" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="14" min="11" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="21" min="16" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1025" min="23" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3060,7 +3068,7 @@
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3075,14 +3083,13 @@
   </sheetPr>
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="52" width="187.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="10.09"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="52" width="185.479591836735"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3108,7 +3115,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -3123,23 +3130,23 @@
   </sheetPr>
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.89"/>
-    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="2" min="2" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="4.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="5" style="0" width="8.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="51.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="8.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="9.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="8.67"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="true" max="2" min="2" style="0" width="0"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="4.45408163265306"/>
+    <col collapsed="false" hidden="false" max="8" min="5" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="50.6224489795918"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="43.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3473,7 +3480,7 @@
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3486,25 +3493,25 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H1048576"/>
+  <dimension ref="A1:H65536"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="H19" activeCellId="0" sqref="H19"/>
+      <selection pane="bottomLeft" activeCell="H22" activeCellId="0" sqref="H22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="74.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="8.67"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.2755102040816"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.8724489795918"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="73.9744897959184"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4053,24 +4060,24 @@
         <v>228</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="22.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="60" t="s">
         <v>229</v>
       </c>
       <c r="B22" s="58" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="C22" s="52" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D22" s="52" t="n">
         <v>1</v>
       </c>
-      <c r="E22" s="61" t="s">
-        <v>166</v>
-      </c>
-      <c r="F22" s="61" t="s">
+      <c r="E22" s="58" t="s">
         <v>198</v>
+      </c>
+      <c r="F22" s="58" t="s">
+        <v>194</v>
       </c>
       <c r="G22" s="43" t="s">
         <v>164</v>
@@ -4079,31 +4086,56 @@
         <v>230</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C23" s="43"/>
-      <c r="D23" s="43"/>
-      <c r="E23" s="61"/>
-      <c r="F23" s="61"/>
-      <c r="G23" s="43"/>
-      <c r="H23" s="63"/>
-    </row>
-    <row r="24" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B24" s="52"/>
+    <row r="23" customFormat="false" ht="22.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="60" t="s">
+        <v>231</v>
+      </c>
+      <c r="B23" s="58" t="s">
+        <v>196</v>
+      </c>
+      <c r="C23" s="52" t="n">
+        <v>0</v>
+      </c>
+      <c r="D23" s="52" t="n">
+        <v>1</v>
+      </c>
+      <c r="E23" s="61" t="s">
+        <v>166</v>
+      </c>
+      <c r="F23" s="61" t="s">
+        <v>198</v>
+      </c>
+      <c r="G23" s="43" t="s">
+        <v>164</v>
+      </c>
+      <c r="H23" s="62" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C24" s="43"/>
       <c r="D24" s="43"/>
       <c r="E24" s="61"/>
       <c r="F24" s="61"/>
       <c r="G24" s="43"/>
-      <c r="H24" s="64"/>
-    </row>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="H24" s="63"/>
+    </row>
+    <row r="25" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B25" s="52"/>
+      <c r="C25" s="43"/>
+      <c r="D25" s="43"/>
+      <c r="E25" s="61"/>
+      <c r="F25" s="61"/>
+      <c r="G25" s="43"/>
+      <c r="H25" s="64"/>
+    </row>
     <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -4118,36 +4150,36 @@
   </sheetPr>
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="52" width="12.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="52" width="18.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="65" width="43.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="52" width="34.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="78.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="8.67"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="52" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="52" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="65" width="42.9285714285714"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="52" width="34.2857142857143"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="77.7551020408163"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="66" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="B1" s="42" t="s">
         <v>79</v>
       </c>
       <c r="C1" s="42" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="D1" s="67" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="E1" s="42" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="F1" s="66" t="s">
         <v>11</v>
@@ -4155,7 +4187,7 @@
     </row>
     <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="B2" s="52" t="n">
         <v>32</v>
@@ -4163,27 +4195,31 @@
       <c r="C2" s="52" t="s">
         <v>164</v>
       </c>
+      <c r="D2" s="0"/>
+      <c r="E2" s="0"/>
       <c r="F2" s="0" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="B3" s="52" t="n">
         <v>32</v>
       </c>
       <c r="C3" s="52" t="s">
-        <v>238</v>
-      </c>
+        <v>240</v>
+      </c>
+      <c r="D3" s="0"/>
+      <c r="E3" s="0"/>
       <c r="F3" s="0" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="B4" s="52" t="n">
         <v>32</v>
@@ -4191,27 +4227,31 @@
       <c r="C4" s="52" t="s">
         <v>169</v>
       </c>
+      <c r="D4" s="0"/>
+      <c r="E4" s="0"/>
       <c r="F4" s="0" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="B5" s="52" t="n">
         <v>32</v>
       </c>
       <c r="C5" s="52" t="s">
-        <v>243</v>
-      </c>
+        <v>245</v>
+      </c>
+      <c r="D5" s="0"/>
+      <c r="E5" s="0"/>
       <c r="F5" s="0" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="58" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="B6" s="52" t="n">
         <v>32</v>
@@ -4220,173 +4260,175 @@
         <v>172</v>
       </c>
       <c r="D6" s="57" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="E6" s="58" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="B7" s="52" t="n">
         <v>32</v>
       </c>
       <c r="C7" s="52" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="D7" s="57" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="E7" s="52" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="43.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="B8" s="52" t="n">
         <v>32</v>
       </c>
       <c r="C8" s="43" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="D8" s="57" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="E8" s="52" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="B9" s="52" t="n">
         <v>32</v>
       </c>
       <c r="C9" s="52" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="D9" s="57" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="E9" s="52" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="43.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="B10" s="52" t="n">
         <v>32</v>
       </c>
       <c r="C10" s="43" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="D10" s="57" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="E10" s="52" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="B11" s="52" t="n">
         <v>32</v>
       </c>
       <c r="C11" s="52" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="D11" s="65" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="E11" s="52" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="B12" s="52" t="n">
         <v>32</v>
       </c>
       <c r="C12" s="52" t="s">
-        <v>275</v>
-      </c>
+        <v>277</v>
+      </c>
+      <c r="D12" s="0"/>
+      <c r="E12" s="0"/>
       <c r="F12" s="0" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="B13" s="52" t="n">
         <v>32</v>
       </c>
       <c r="C13" s="52" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="D13" s="65" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="E13" s="52" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="B14" s="52" t="n">
         <v>32</v>
       </c>
       <c r="C14" s="52" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="D14" s="65" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="E14" s="52" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -4401,27 +4443,27 @@
   </sheetPr>
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="74.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="33" width="74.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="8.67"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.765306122449"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.7908163265306"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="73.4336734693878"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="33" width="73.4336734693878"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="59" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="B1" s="42" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="C1" s="42" t="s">
         <v>105</v>
@@ -4430,7 +4472,7 @@
         <v>79</v>
       </c>
       <c r="E1" s="42" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="F1" s="55" t="s">
         <v>11</v>
@@ -4438,10 +4480,10 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>28</v>
@@ -4453,15 +4495,15 @@
         <v>164</v>
       </c>
       <c r="F2" s="33" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>28</v>
@@ -4470,18 +4512,18 @@
         <v>4</v>
       </c>
       <c r="E3" s="43" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="F3" s="33" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>28</v>
@@ -4493,15 +4535,15 @@
         <v>169</v>
       </c>
       <c r="F4" s="33" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>28</v>
@@ -4510,18 +4552,18 @@
         <v>4</v>
       </c>
       <c r="E5" s="43" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="F5" s="33" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>28</v>
@@ -4533,15 +4575,15 @@
         <v>172</v>
       </c>
       <c r="F6" s="33" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>28</v>
@@ -4550,18 +4592,18 @@
         <v>4</v>
       </c>
       <c r="E7" s="43" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="F7" s="33" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="B8" s="34" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>0</v>
@@ -4570,18 +4612,18 @@
         <v>16</v>
       </c>
       <c r="E8" s="43" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="F8" s="33" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>28</v>
@@ -4590,18 +4632,18 @@
         <v>4</v>
       </c>
       <c r="E9" s="43" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="F9" s="33" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="B10" s="34" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>0</v>
@@ -4610,18 +4652,18 @@
         <v>16</v>
       </c>
       <c r="E10" s="43" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="F10" s="33" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>28</v>
@@ -4630,18 +4672,18 @@
         <v>4</v>
       </c>
       <c r="E11" s="43" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="F11" s="33" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="B12" s="34" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>0</v>
@@ -4650,18 +4692,18 @@
         <v>16</v>
       </c>
       <c r="E12" s="43" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="F12" s="33" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>28</v>
@@ -4670,18 +4712,18 @@
         <v>4</v>
       </c>
       <c r="E13" s="43" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="F13" s="33" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="B14" s="34" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="C14" s="34" t="n">
         <v>28</v>
@@ -4690,18 +4732,18 @@
         <v>4</v>
       </c>
       <c r="E14" s="43" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="F14" s="33" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="B15" s="34" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="C15" s="34" t="n">
         <v>0</v>
@@ -4710,18 +4752,18 @@
         <v>8</v>
       </c>
       <c r="E15" s="43" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="F15" s="33" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="B16" s="34" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="C16" s="34" t="n">
         <v>28</v>
@@ -4730,18 +4772,18 @@
         <v>4</v>
       </c>
       <c r="E16" s="43" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="F16" s="33" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="B17" s="34" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="C17" s="34" t="n">
         <v>28</v>
@@ -4750,18 +4792,18 @@
         <v>4</v>
       </c>
       <c r="E17" s="43" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="F17" s="33" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="B18" s="34" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="C18" s="34" t="n">
         <v>27</v>
@@ -4770,18 +4812,18 @@
         <v>1</v>
       </c>
       <c r="E18" s="43" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="F18" s="33" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="B19" s="34" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="C19" s="34" t="n">
         <v>0</v>
@@ -4790,18 +4832,18 @@
         <v>24</v>
       </c>
       <c r="E19" s="43" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="F19" s="33" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="B20" s="34" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="C20" s="34" t="n">
         <v>28</v>
@@ -4810,18 +4852,18 @@
         <v>4</v>
       </c>
       <c r="E20" s="43" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="F20" s="57" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="B21" s="34" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="C21" s="34" t="n">
         <v>27</v>
@@ -4830,18 +4872,18 @@
         <v>1</v>
       </c>
       <c r="E21" s="43" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="F21" s="33" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="B22" s="34" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="C22" s="34" t="n">
         <v>0</v>
@@ -4850,16 +4892,16 @@
         <v>16</v>
       </c>
       <c r="E22" s="43" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="F22" s="33" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>